<commit_message>
js 8 praktikum 3
</commit_message>
<xml_diff>
--- a/public/template_user.xlsx
+++ b/public/template_user.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6931FAB8-1B01-4184-977F-E377B5CDA3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BEBE7E-16B2-4211-912A-273677886901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7C859632-E94E-4203-B759-DEEF37154D4F}"/>
+    <workbookView xWindow="4800" yWindow="2810" windowWidth="14400" windowHeight="7270" xr2:uid="{7C859632-E94E-4203-B759-DEEF37154D4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>level_id</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>intan</t>
+  </si>
+  <si>
+    <t>user_id</t>
   </si>
 </sst>
 </file>
@@ -429,9 +429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{099B01B6-ED29-4711-87F5-8A322924FE5D}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -443,16 +441,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -460,10 +458,10 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>12345</v>
@@ -474,10 +472,10 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>12345</v>
@@ -488,10 +486,10 @@
         <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>12345</v>
@@ -502,10 +500,10 @@
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>12345</v>
@@ -516,10 +514,10 @@
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>12345</v>

</xml_diff>